<commit_message>
Modificar plantilla de detalle a reporte de tiempo
</commit_message>
<xml_diff>
--- a/application/includes/phpexcel/plantillas/Timesheets.xlsx
+++ b/application/includes/phpexcel/plantillas/Timesheets.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Erp\application\includes\phpexcel\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89536660-8CBC-46BC-B16C-3F67CBA6744F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128D3D07-E7C5-44A3-BE36-3A1780634790}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EF848CFC-D104-4789-9425-9CD2D7053172}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nombre</t>
   </si>
@@ -55,6 +56,9 @@
   </si>
   <si>
     <t>Descripción</t>
+  </si>
+  <si>
+    <t>Ususario</t>
   </si>
 </sst>
 </file>
@@ -447,9 +451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3B2CE3-A00E-40CB-9111-73C5522790A7}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -492,4 +494,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD4F4FE3-9ABF-4385-9AF9-24D432527678}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="2" max="16384" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>